<commit_message>
rPDM - Started on board layout
</commit_message>
<xml_diff>
--- a/LV/RPDM v2/pth_pad_size_calcs.xlsx
+++ b/LV/RPDM v2/pth_pad_size_calcs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshsmedley/Documents/GitHub/UOW-Motorsport-Team/KiCad/LV/RPDM v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21829011-0362-5C41-A2D4-7D76C6AE2680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C855A6C7-9715-F74F-93B9-F3776A373244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="28720" windowHeight="17500" xr2:uid="{3F7F42D3-FEA5-BB4F-8636-B890E0F7E300}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,13 +455,15 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>1.57</v>
+      </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>1.6</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>1.1099999999999999</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>